<commit_message>
add framework for e2e  test
</commit_message>
<xml_diff>
--- a/data/cahier_recette.xlsx
+++ b/data/cahier_recette.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/olivier/Documents/formation/CESI/CUBES/PROJET 1/LIVRABLE_3/good_food_2.0/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDD54120-D9A7-B34D-AB89-FC460C549A55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F000066-CC71-BF4E-9CE6-89C82084E238}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="0" windowWidth="28040" windowHeight="17440" xr2:uid="{8491249C-8AC8-C34D-A75D-4727B12E9C02}"/>
+    <workbookView xWindow="380" yWindow="0" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{8491249C-8AC8-C34D-A75D-4727B12E9C02}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
+    <sheet name="Scenario" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>developpeur</t>
   </si>
@@ -46,15 +47,89 @@
   </si>
   <si>
     <t>donnée de test</t>
+  </si>
+  <si>
+    <t>step</t>
+  </si>
+  <si>
+    <t>l'utilisateur se connecte à localhost</t>
+  </si>
+  <si>
+    <t>impact</t>
+  </si>
+  <si>
+    <t>la page d'accueil s'ouvre</t>
+  </si>
+  <si>
+    <t>critère</t>
+  </si>
+  <si>
+    <t xml:space="preserve">les deux bouttons son présent
+</t>
+  </si>
+  <si>
+    <t>le titre est présent.</t>
+  </si>
+  <si>
+    <t>L'image est chargée</t>
+  </si>
+  <si>
+    <t>l'utilisateur clique sur "Yes, connect to my account"</t>
+  </si>
+  <si>
+    <t>la page login est ouverte</t>
+  </si>
+  <si>
+    <t>le  boutton Home est présent</t>
+  </si>
+  <si>
+    <t>l'input enter your login est présent</t>
+  </si>
+  <si>
+    <t>description test</t>
+  </si>
+  <si>
+    <t>l'utilisateur clique sur "Connect"</t>
+  </si>
+  <si>
+    <t>uen pop-up apparait</t>
+  </si>
+  <si>
+    <t>Le titre 'Athentication failed" est présent</t>
+  </si>
+  <si>
+    <t>le boutton "Close est présent"</t>
+  </si>
+  <si>
+    <t>le text login/password est présent</t>
+  </si>
+  <si>
+    <t>la requete http "POST: http://localhost:5001/auth"  return 400</t>
+  </si>
+  <si>
+    <t>l'utilisateur tente de se connecter à l'application, il valide mais n'a entré aucun paramètre. Une Pop up apparaît.</t>
+  </si>
+  <si>
+    <t>l'input enter your password est présent</t>
+  </si>
+  <si>
+    <t>l'url est localhost:4200/login</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -81,10 +156,25 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -402,8 +492,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B2FB7F1-C22F-5743-B0BF-517425E1A1F7}">
   <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -432,4 +522,149 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05AC58C3-F662-1A48-B1A2-904BC4583732}">
+  <dimension ref="A1:D12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="32.1640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="43.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="27.6640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="38.1640625" style="4" customWidth="1"/>
+    <col min="5" max="16384" width="10.83203125" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A3" s="3"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A4" s="3"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A5" s="3"/>
+      <c r="C5" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" s="3"/>
+      <c r="B6" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="5"/>
+      <c r="D6" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A7" s="3"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A8" s="3"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A9" s="3"/>
+      <c r="B9" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A10" s="3"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A11" s="3"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A12" s="3"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="A2:A12"/>
+    <mergeCell ref="C5:C8"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="C2:C4"/>
+    <mergeCell ref="C9:C12"/>
+    <mergeCell ref="B9:B12"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>